<commit_message>
double everywhere + N et T parametrized + lots of stuff to compute
</commit_message>
<xml_diff>
--- a/RS-IBCF-2016/readme/ibcf.xlsx
+++ b/RS-IBCF-2016/readme/ibcf.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t>neighbourhoodSize</t>
   </si>
@@ -85,9 +85,6 @@
     <t>RMSE (true rating = 5): 1,239617</t>
   </si>
   <si>
-    <t>coverage: 99,20%</t>
-  </si>
-  <si>
     <t>RMSE (true rating = 1): 2,193794</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
   </si>
   <si>
     <t>RMSE (true rating = 5): 1,589067</t>
-  </si>
-  <si>
-    <t>coverage: 44,19%</t>
   </si>
   <si>
     <t>RMSE (true rating = 1): 2,139186</t>
@@ -121,9 +115,6 @@
     <t>RMSE (true rating = 5): 1,321695</t>
   </si>
   <si>
-    <t>coverage: 96,78%</t>
-  </si>
-  <si>
     <t>RMSE (true rating = 1): 2,256613</t>
   </si>
   <si>
@@ -139,28 +130,10 @@
     <t>RMSE (true rating = 5): 1,407479</t>
   </si>
   <si>
-    <t>coverage: 24,65%</t>
-  </si>
-  <si>
     <t>synthese</t>
   </si>
   <si>
     <t>RMSE</t>
-  </si>
-  <si>
-    <t>1,092697</t>
-  </si>
-  <si>
-    <t>1,342428</t>
-  </si>
-  <si>
-    <t>1,116123</t>
-  </si>
-  <si>
-    <t>1,202419</t>
-  </si>
-  <si>
-    <t>Metric</t>
   </si>
   <si>
     <t>CosineMetric</t>
@@ -176,6 +149,15 @@
   </si>
   <si>
     <t>JaccardMetric</t>
+  </si>
+  <si>
+    <t>michael</t>
+  </si>
+  <si>
+    <t>Coverage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coverage: </t>
   </si>
 </sst>
 </file>
@@ -1388,6 +1370,744 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'exp3'!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RMSE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'exp3'!$I$2:$I$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>CosineMetric</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PearsonMetric</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>PearsonSignifianceWeightMetric</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>JaccardMetric</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'exp3'!$J$2:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.09269670288217</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.34242830804724</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.11612349179624</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.20241944947996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="75"/>
+        <c:axId val="-2059919952"/>
+        <c:axId val="-2058808576"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2059919952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2058808576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2058808576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2059919952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="accent1">
+              <a:lumMod val="5000"/>
+              <a:lumOff val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="74000">
+            <a:schemeClr val="accent1">
+              <a:lumMod val="45000"/>
+              <a:lumOff val="55000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="83000">
+            <a:schemeClr val="accent1">
+              <a:lumMod val="45000"/>
+              <a:lumOff val="55000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="accent1">
+              <a:lumMod val="30000"/>
+              <a:lumOff val="70000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="1"/>
+      </a:gradFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'exp3'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Coverage</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'exp3'!$I$2:$I$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>CosineMetric</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PearsonMetric</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>PearsonSignifianceWeightMetric</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>JaccardMetric</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'exp3'!$K$2:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>99.1953252227224</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44.1900565188236</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96.78130089088989</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.647954784941</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="75"/>
+        <c:axId val="-2057633392"/>
+        <c:axId val="-2037314160"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2057633392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2037314160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2037314160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2057633392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -2200,7 +2920,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -3182,6 +3902,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4215,7 +5015,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4242,8 +5042,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4344,7 +5144,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -4376,6 +5176,1012 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
@@ -4730,7 +6536,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5316,6 +7122,71 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3517900</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Graphique 11"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Graphique 13"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5923,10 +7794,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5935,26 +7806,29 @@
     <col min="9" max="9" width="30.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>38</v>
       </c>
-      <c r="I1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s">
-        <v>40</v>
+      <c r="B2">
+        <v>1.0926967028821699</v>
       </c>
       <c r="G2" t="str">
         <f>A1</f>
@@ -5964,46 +7838,64 @@
         <f>A1</f>
         <v>CosineMetric</v>
       </c>
-      <c r="J2" t="str">
+      <c r="J2">
         <f>B2</f>
-        <v>1,092697</v>
+        <v>1.0926967028821699</v>
+      </c>
+      <c r="K2">
+        <f>B8</f>
+        <v>99.195325222722403</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="G3" t="str">
         <f>A8</f>
-        <v>coverage: 99,20%</v>
+        <v xml:space="preserve">coverage: </v>
+      </c>
+      <c r="H3">
+        <v>100</v>
       </c>
       <c r="I3" t="str">
         <f>A9</f>
         <v>PearsonMetric</v>
       </c>
-      <c r="J3" t="str">
+      <c r="J3">
         <f>B10</f>
-        <v>1,342428</v>
+        <v>1.3424283080472399</v>
+      </c>
+      <c r="K3">
+        <f>B16</f>
+        <v>44.190056518823603</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" t="str">
-        <f>A2</f>
-        <v xml:space="preserve">RMSE: </v>
+      <c r="G4">
+        <f>B2</f>
+        <v>1.0926967028821699</v>
+      </c>
+      <c r="H4">
+        <v>0.9</v>
       </c>
       <c r="I4" t="str">
         <f>A17</f>
         <v>PearsonSignifianceWeightMetric</v>
       </c>
-      <c r="J4" t="str">
+      <c r="J4">
         <f>B18</f>
-        <v>1,116123</v>
+        <v>1.1161234917962399</v>
+      </c>
+      <c r="K4">
+        <f>B24</f>
+        <v>96.781300890889895</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -6015,201 +7907,219 @@
         <f>A25</f>
         <v>JaccardMetric</v>
       </c>
-      <c r="J5" t="str">
+      <c r="J5">
         <f>B26</f>
-        <v>1,202419</v>
+        <v>1.20241944947996</v>
+      </c>
+      <c r="K5">
+        <f>B32</f>
+        <v>24.647954784941</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="G6" t="str">
         <f>A16</f>
-        <v>coverage: 44,19%</v>
+        <v xml:space="preserve">coverage: </v>
+      </c>
+      <c r="H6">
+        <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="G7" t="str">
-        <f>A10</f>
-        <v xml:space="preserve">RMSE: </v>
+      <c r="G7">
+        <f>B10</f>
+        <v>1.3424283080472399</v>
+      </c>
+      <c r="H7">
+        <v>1.2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>43</v>
+      </c>
+      <c r="B8">
+        <v>99.195325222722403</v>
       </c>
       <c r="G8" t="str">
         <f>A17</f>
         <v>PearsonSignifianceWeightMetric</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="G9" t="str">
         <f>A24</f>
-        <v>coverage: 96,78%</v>
-      </c>
-      <c r="I9" t="str">
-        <f>I2</f>
-        <v>CosineMetric</v>
-      </c>
-      <c r="J9" t="str">
-        <f>I3</f>
-        <v>PearsonMetric</v>
+        <v xml:space="preserve">coverage: </v>
+      </c>
+      <c r="H9">
+        <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" t="str">
-        <f>A10</f>
-        <v xml:space="preserve">RMSE: </v>
-      </c>
-      <c r="I10" t="str">
-        <f>J2</f>
-        <v>1,092697</v>
-      </c>
-      <c r="J10" t="str">
-        <f>J3</f>
-        <v>1,342428</v>
+        <v>38</v>
+      </c>
+      <c r="B10">
+        <v>1.3424283080472399</v>
+      </c>
+      <c r="G10">
+        <f>B10</f>
+        <v>1.3424283080472399</v>
+      </c>
+      <c r="H10">
+        <v>1.2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G11" t="str">
         <f>A25</f>
         <v>JaccardMetric</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G12" t="str">
         <f>A32</f>
-        <v>coverage: 24,65%</v>
+        <v xml:space="preserve">coverage: </v>
+      </c>
+      <c r="H12">
+        <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13">
+        <f>B26</f>
+        <v>1.20241944947996</v>
+      </c>
+      <c r="H13">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="G13" t="str">
-        <f>A26</f>
-        <v xml:space="preserve">RMSE: </v>
-      </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>43</v>
+      </c>
+      <c r="B16">
+        <v>44.190056518823603</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="B18">
+        <v>1.1161234917962399</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>43</v>
+      </c>
+      <c r="B24">
+        <v>96.781300890889895</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="B26">
+        <v>1.20241944947996</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="B32">
+        <v>24.647954784941</v>
       </c>
     </row>
   </sheetData>
@@ -6218,6 +8128,7 @@
   <ignoredErrors>
     <ignoredError sqref="I3" formula="1"/>
   </ignoredErrors>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>